<commit_message>
Added ability to add more input
</commit_message>
<xml_diff>
--- a/data/stations_metadata.xlsx
+++ b/data/stations_metadata.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+  <si>
+    <t>river_name</t>
+  </si>
+  <si>
+    <t>station_name</t>
+  </si>
   <si>
     <t>station_code</t>
   </si>
@@ -22,24 +28,21 @@
     <t>station_id</t>
   </si>
   <si>
-    <t>station_name</t>
-  </si>
-  <si>
-    <t>river_name</t>
+    <t>station_kodas</t>
+  </si>
+  <si>
+    <t>x_coord</t>
+  </si>
+  <si>
+    <t>y_coord</t>
+  </si>
+  <si>
+    <t>roughness_n</t>
   </si>
   <si>
     <t>basin_name</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>station_level_cm</t>
-  </si>
-  <si>
     <t>datum_offset_cm</t>
   </si>
   <si>
@@ -49,46 +52,97 @@
     <t>max_level_cm</t>
   </si>
   <si>
-    <t>roughness_n</t>
+    <t>Merkys</t>
+  </si>
+  <si>
+    <t>Nemunas</t>
+  </si>
+  <si>
+    <t>Verknė</t>
+  </si>
+  <si>
+    <t>Šešupė</t>
+  </si>
+  <si>
+    <t>Nemuno atšaka Atmata</t>
+  </si>
+  <si>
+    <t>Puvočiai</t>
+  </si>
+  <si>
+    <t>Druskininkai</t>
+  </si>
+  <si>
+    <t>Verbyliškės</t>
+  </si>
+  <si>
+    <t>Nemunaičiai</t>
+  </si>
+  <si>
+    <t>Jašiūnai</t>
+  </si>
+  <si>
+    <t>Kudirkos Naumiestis</t>
+  </si>
+  <si>
+    <t>Rusnė</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>769</t>
+  </si>
+  <si>
+    <t>5101LT</t>
+  </si>
+  <si>
+    <t>5102LT</t>
+  </si>
+  <si>
+    <t>5103LT</t>
+  </si>
+  <si>
+    <t>5104LT</t>
+  </si>
+  <si>
+    <t>5105LT</t>
+  </si>
+  <si>
+    <t>5106LT</t>
   </si>
   <si>
     <t>60004LT</t>
   </si>
   <si>
-    <t>Rusnė</t>
-  </si>
-  <si>
-    <t>Puvočiai</t>
-  </si>
-  <si>
-    <t>Druskininkai</t>
-  </si>
-  <si>
-    <t>Verbyliškės</t>
-  </si>
-  <si>
-    <t>Nemajūnai</t>
-  </si>
-  <si>
-    <t>Jašiūnai</t>
-  </si>
-  <si>
-    <t>Kudirkos Naumiestis</t>
-  </si>
-  <si>
-    <t>Nemuno atšaka Atmata</t>
-  </si>
-  <si>
-    <t>Merkys</t>
-  </si>
-  <si>
-    <t>Nemunas</t>
-  </si>
-  <si>
-    <t>Verknė</t>
-  </si>
-  <si>
-    <t>Šešupė</t>
+    <t>Nemunas-Merkys</t>
+  </si>
+  <si>
+    <t>Nemunas-Main</t>
+  </si>
+  <si>
+    <t>Nemunas-Verkne</t>
+  </si>
+  <si>
+    <t>Nemunas-Sesupe</t>
+  </si>
+  <si>
+    <t>Nemunas-Delta</t>
   </si>
 </sst>
 </file>
@@ -494,113 +548,266 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>769</v>
+      <c r="B2" t="s">
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>5101</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F2">
-        <v>333694</v>
+        <v>575000</v>
       </c>
       <c r="G2">
-        <v>6132670</v>
+        <v>5998000</v>
       </c>
       <c r="H2">
-        <v>227.1</v>
-      </c>
-      <c r="I2">
-        <v>-1.56</v>
+        <v>0.04</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>850</v>
       </c>
     </row>
     <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>5102</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>568500</v>
+      </c>
+      <c r="G3">
+        <v>5992000</v>
       </c>
       <c r="H3">
-        <v>500.2</v>
+        <v>0.038</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>5103</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>521000</v>
+      </c>
+      <c r="G4">
+        <v>6032000</v>
       </c>
       <c r="H4">
-        <v>40.1</v>
+        <v>0.042</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>700</v>
       </c>
     </row>
     <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>5104</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="F5">
+        <v>540500</v>
+      </c>
+      <c r="G5">
+        <v>6042000</v>
       </c>
       <c r="H5">
-        <v>142.8</v>
+        <v>0.038</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>1100</v>
       </c>
     </row>
     <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>5105</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>583500</v>
+      </c>
+      <c r="G6">
+        <v>6029000</v>
       </c>
       <c r="H6">
-        <v>50.6</v>
+        <v>0.04</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>30</v>
+      </c>
+      <c r="L6">
+        <v>800</v>
       </c>
     </row>
     <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>5106</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="F7">
+        <v>409000</v>
+      </c>
+      <c r="G7">
+        <v>6022000</v>
       </c>
       <c r="H7">
-        <v>142.7</v>
+        <v>0.045</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>40</v>
+      </c>
+      <c r="L7">
+        <v>950</v>
       </c>
     </row>
     <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>769</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>333694</v>
+      </c>
+      <c r="G8">
+        <v>6132670</v>
       </c>
       <c r="H8">
-        <v>101.7</v>
+        <v>0.03</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8">
+        <v>-1.56</v>
+      </c>
+      <c r="K8">
+        <v>-100</v>
+      </c>
+      <c r="L8">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>